<commit_message>
committing before messing with internal layers
</commit_message>
<xml_diff>
--- a/IV_Array/Project Outputs/BOM/Bill of Materials-IV_Array.xlsx
+++ b/IV_Array/Project Outputs/BOM/Bill of Materials-IV_Array.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\college\UROP_S2022\IV_Array\Project Outputs\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DC0B0250-854D-477B-B47B-AED483EC164C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F7691F50-84E4-4B5C-8332-AD26764E8576}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8964" xr2:uid="{FD6C4212-7019-46B8-87EE-AA7E47A7D427}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8964" xr2:uid="{B8A0957F-1709-4EA6-AB0D-2C639CDE93C6}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-IV_Array" sheetId="1" r:id="rId1"/>
@@ -1000,7 +1000,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D0635D3-9E2D-4697-937E-A951385780BE}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02AB1F0F-A593-4F9E-B4EB-988FC6691652}">
   <dimension ref="A1:H42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
increased via size from 20 to 24 mils
</commit_message>
<xml_diff>
--- a/IV_Array/Project Outputs/BOM/Bill of Materials-IV_Array.xlsx
+++ b/IV_Array/Project Outputs/BOM/Bill of Materials-IV_Array.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\college\UROP_S2022\IV_Array\Project Outputs\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F7691F50-84E4-4B5C-8332-AD26764E8576}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{475A4CE4-6019-4078-B44C-E2EC9F45DEEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8964" xr2:uid="{B8A0957F-1709-4EA6-AB0D-2C639CDE93C6}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8964" xr2:uid="{AE2769DD-2200-4998-9710-B4D7EB658553}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-IV_Array" sheetId="1" r:id="rId1"/>
@@ -1000,7 +1000,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02AB1F0F-A593-4F9E-B4EB-988FC6691652}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A7C3B78-5386-4A81-929D-100C4DD0BD59}">
   <dimension ref="A1:H42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>